<commit_message>
Pushed the previous repository to the new repository
</commit_message>
<xml_diff>
--- a/6 Detect linguistic inconsistency/skip/xgboost_fasttext.xlsx
+++ b/6 Detect linguistic inconsistency/skip/xgboost_fasttext.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Postdoc\projects\deepiac_extension\skip\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>shell</t>
   </si>
@@ -71,13 +76,22 @@
   </si>
   <si>
     <t>roc_auc</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Worst</t>
+  </si>
+  <si>
+    <t>best</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -125,13 +139,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -140,6 +169,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -186,7 +223,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,9 +255,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,6 +290,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -427,14 +466,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,66 +506,84 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.955</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="C2">
-        <v>0.922</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="D2">
-        <v>0.946</v>
+        <v>0.94599999999999995</v>
       </c>
       <c r="E2">
-        <v>0.9419999999999999</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="F2">
-        <v>0.959</v>
+        <v>0.95899999999999996</v>
       </c>
       <c r="G2">
         <v>0.96</v>
       </c>
       <c r="H2">
-        <v>0.926</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="I2">
-        <v>0.974</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="J2">
-        <v>0.979</v>
+        <v>0.97899999999999998</v>
       </c>
       <c r="K2">
-        <v>0.924</v>
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="M2">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="N2">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="O2">
+        <v>0.94869999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.952</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="C3">
-        <v>0.927</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="D3">
-        <v>0.9429999999999999</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="E3">
-        <v>0.977</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="F3">
-        <v>0.982</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="G3">
-        <v>0.973</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="H3">
-        <v>0.923</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="I3">
         <v>0.98</v>
@@ -533,164 +592,209 @@
         <v>0.99</v>
       </c>
       <c r="K3">
-        <v>0.9370000000000001</v>
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="M3">
+        <v>0.99</v>
+      </c>
+      <c r="N3">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="O3">
+        <v>0.95840000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.956</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="C4">
-        <v>0.906</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="D4">
-        <v>0.954</v>
+        <v>0.95399999999999996</v>
       </c>
       <c r="E4">
-        <v>0.901</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="F4">
-        <v>0.9350000000000001</v>
+        <v>0.93500000000000005</v>
       </c>
       <c r="G4">
-        <v>0.947</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="H4">
-        <v>0.929</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="I4">
         <v>0.96</v>
       </c>
       <c r="J4">
-        <v>0.969</v>
+        <v>0.96899999999999997</v>
       </c>
       <c r="K4">
-        <v>0.914</v>
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="M4">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="N4">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="O4">
+        <v>0.93710000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5">
-        <v>0.954</v>
+        <v>0.95399999999999996</v>
       </c>
       <c r="C5">
-        <v>0.916</v>
+        <v>0.91600000000000004</v>
       </c>
       <c r="D5">
-        <v>0.948</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="E5">
-        <v>0.9379999999999999</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="F5">
-        <v>0.958</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="G5">
         <v>0.96</v>
       </c>
       <c r="H5">
-        <v>0.926</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="I5">
         <v>0.97</v>
       </c>
       <c r="J5">
-        <v>0.979</v>
+        <v>0.97899999999999998</v>
       </c>
       <c r="K5">
-        <v>0.925</v>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="M5">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="N5">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="O5">
+        <v>0.94740000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B6">
-        <v>0.959</v>
+        <v>0.95899999999999996</v>
       </c>
       <c r="C6">
-        <v>0.918</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="D6">
-        <v>0.949</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="E6">
-        <v>0.913</v>
+        <v>0.91300000000000003</v>
       </c>
       <c r="F6">
-        <v>0.9379999999999999</v>
+        <v>0.93799999999999994</v>
       </c>
       <c r="G6">
-        <v>0.948</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="H6">
-        <v>0.929</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="I6">
-        <v>0.969</v>
+        <v>0.96899999999999997</v>
       </c>
       <c r="J6">
-        <v>0.969</v>
+        <v>0.96899999999999997</v>
       </c>
       <c r="K6">
-        <v>0.911</v>
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="M6">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="N6">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="O6">
+        <v>0.94030000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7">
-        <v>0.955</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="C7">
-        <v>0.9360000000000001</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="D7">
-        <v>0.9370000000000001</v>
+        <v>0.93700000000000006</v>
       </c>
       <c r="E7">
         <v>0.98</v>
       </c>
       <c r="F7">
-        <v>0.983</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="G7">
-        <v>0.973</v>
+        <v>0.97299999999999998</v>
       </c>
       <c r="H7">
-        <v>0.923</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="I7">
-        <v>0.984</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="J7">
         <v>0.99</v>
       </c>
       <c r="K7">
-        <v>0.9350000000000001</v>
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="M7">
+        <v>0.99</v>
+      </c>
+      <c r="N7">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="O7">
+        <v>0.95960000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B8">
-        <v>0.957</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="C8">
-        <v>0.927</v>
+        <v>0.92700000000000005</v>
       </c>
       <c r="D8">
-        <v>0.9429999999999999</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="E8">
-        <v>0.945</v>
+        <v>0.94499999999999995</v>
       </c>
       <c r="F8">
         <v>0.96</v>
@@ -699,86 +803,113 @@
         <v>0.96</v>
       </c>
       <c r="H8">
-        <v>0.926</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="I8">
-        <v>0.977</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="J8">
-        <v>0.979</v>
+        <v>0.97899999999999998</v>
       </c>
       <c r="K8">
-        <v>0.923</v>
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="M8">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="N8">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="O8">
+        <v>0.94969999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9">
-        <v>0.911</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="C9">
-        <v>0.844</v>
+        <v>0.84399999999999997</v>
       </c>
       <c r="D9">
-        <v>0.892</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="E9">
-        <v>0.885</v>
+        <v>0.88500000000000001</v>
       </c>
       <c r="F9">
-        <v>0.919</v>
+        <v>0.91900000000000004</v>
       </c>
       <c r="G9">
-        <v>0.921</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="H9">
-        <v>0.852</v>
+        <v>0.85199999999999998</v>
       </c>
       <c r="I9">
-        <v>0.947</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="J9">
-        <v>0.959</v>
+        <v>0.95899999999999996</v>
       </c>
       <c r="K9">
-        <v>0.848</v>
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="M9">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="N9">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="O9">
+        <v>0.89780000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10">
-        <v>0.955</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="C10">
-        <v>0.921</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="D10">
-        <v>0.946</v>
+        <v>0.94599999999999995</v>
       </c>
       <c r="E10">
-        <v>0.9409999999999999</v>
+        <v>0.94099999999999995</v>
       </c>
       <c r="F10">
-        <v>0.959</v>
+        <v>0.95899999999999996</v>
       </c>
       <c r="G10">
         <v>0.96</v>
       </c>
       <c r="H10">
-        <v>0.926</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="I10">
-        <v>0.972</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="J10">
-        <v>0.979</v>
+        <v>0.97899999999999998</v>
       </c>
       <c r="K10">
-        <v>0.924</v>
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="M10">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="N10">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="O10">
+        <v>0.94830000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>